<commit_message>
Swapped LM386 inputs, tweaked PCB layout, updated BOM
</commit_message>
<xml_diff>
--- a/Twin-T_Code_Practice_Oscillator_Rev(A)_SystemBOM.xlsx
+++ b/Twin-T_Code_Practice_Oscillator_Rev(A)_SystemBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Doc\JAB\Projects\Morse_Oscillator\_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47186F57-1D8C-4660-B625-7B18B5A052B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AF7E39-AAC7-479E-A5D9-9702E8C55DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4350" yWindow="1560" windowWidth="15180" windowHeight="14670" activeTab="1" xr2:uid="{7B04C32E-1E32-4CC1-8C2E-05A29627A4DD}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Enclosure" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PCB!$A$1:$N$34</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Enclosure!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PCB!$1:$1</definedName>
   </definedNames>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="252">
   <si>
     <t>Sourced</t>
   </si>
@@ -236,51 +237,30 @@
     <t>J1</t>
   </si>
   <si>
-    <t>BATT</t>
-  </si>
-  <si>
     <t>BE_Conn_HDR_SIP-2</t>
   </si>
   <si>
     <t>J3</t>
   </si>
   <si>
-    <t>PITCH</t>
-  </si>
-  <si>
     <t>J5</t>
   </si>
   <si>
-    <t>KEY</t>
-  </si>
-  <si>
     <t>J7</t>
   </si>
   <si>
-    <t>SPKR</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
-    <t>DC IN</t>
-  </si>
-  <si>
     <t>BE_Conn_HDR_SIP-3</t>
   </si>
   <si>
     <t>J4</t>
   </si>
   <si>
-    <t>VOLUME</t>
-  </si>
-  <si>
     <t>J6</t>
   </si>
   <si>
-    <t>PHONES</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -572,9 +552,6 @@
     <t>GF0778B</t>
   </si>
   <si>
-    <t>Potentiometer, 10k Ohms, Linear Taper, with Switch</t>
-  </si>
-  <si>
     <t>CTS</t>
   </si>
   <si>
@@ -582,9 +559,6 @@
   </si>
   <si>
     <t>Volume control and power</t>
-  </si>
-  <si>
-    <t>Potentiometer, 10k Ohms, Reverse Logrithmic Taper</t>
   </si>
   <si>
     <t>P160KNP-0FC25C10K</t>
@@ -709,12 +683,6 @@
     <t>Washer, Flat, Regular, #4</t>
   </si>
   <si>
-    <t>Washer, Flat, Narrow, #6</t>
-  </si>
-  <si>
-    <t>Washer, Flat, Narrow, #4</t>
-  </si>
-  <si>
     <t>For mounting Item 12 (PCB) and Item 7 (Battery Box)</t>
   </si>
   <si>
@@ -736,18 +704,9 @@
     <t>ft.</t>
   </si>
   <si>
-    <t>For wiring the front potentiometers to the PCB</t>
-  </si>
-  <si>
-    <t>Wire, Multiconductor, Jacketed and Shielded, 1 Pair, 26AWG</t>
-  </si>
-  <si>
     <t>A/R</t>
   </si>
   <si>
-    <t>Wire, Single Conductor, Stranded, 22 AWG</t>
-  </si>
-  <si>
     <t>For wiring the Key and Headphone Jacks to the PCB.</t>
   </si>
   <si>
@@ -778,9 +737,6 @@
     <t>For wiring the Speaker, Battery and DC Input Jacks to the PCB.</t>
   </si>
   <si>
-    <t>Wire, Single Conductor, Stranded, 26 AWG</t>
-  </si>
-  <si>
     <t>16-02-1113</t>
   </si>
   <si>
@@ -791,6 +747,48 @@
   </si>
   <si>
     <t>For wiring J3-J6 (Key Jack, Phones Jack, Pitch Pot, Volume Pot)</t>
+  </si>
+  <si>
+    <t>"BATT"</t>
+  </si>
+  <si>
+    <t>"PITCH"</t>
+  </si>
+  <si>
+    <t>"KEY"</t>
+  </si>
+  <si>
+    <t>"SPKR"</t>
+  </si>
+  <si>
+    <t>"DC IN"</t>
+  </si>
+  <si>
+    <t>"VOLUME"</t>
+  </si>
+  <si>
+    <t>"PHONES"</t>
+  </si>
+  <si>
+    <t>Potentiometer, 10k Ohms, Reverse Logrithmic Taper, 6mm dia Shaft</t>
+  </si>
+  <si>
+    <t>Potentiometer, 10k Ohms, Linear Taper, with Switch, 6mm dia Shaft</t>
+  </si>
+  <si>
+    <t>Wire, Multiconductor, Jacketed and Shielded, 1 Pair, 26AWG or 28AWG</t>
+  </si>
+  <si>
+    <t>For wiring the front potentiometers to the PCB. (cable example: Mogami 2697)</t>
+  </si>
+  <si>
+    <t>Wire, Single Conductor, Insulated, Stranded, 22 AWG</t>
+  </si>
+  <si>
+    <t>Wire, Single Conductor, Insulated, Stranded, 26 AWG</t>
+  </si>
+  <si>
+    <t>Washer, Flat, Regular, #6</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1212,8 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28:E31"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1222,7 @@
     <col min="2" max="2" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="0" style="5" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="0" style="5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1232,17 +1230,17 @@
     <col min="11" max="11" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="31.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="0.42578125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="33.28515625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="2.28515625" style="5" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -1260,25 +1258,25 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -1298,25 +1296,25 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1336,25 +1334,25 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
@@ -1374,28 +1372,28 @@
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1415,25 +1413,25 @@
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1453,25 +1451,25 @@
         <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1491,25 +1489,25 @@
         <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
@@ -1529,28 +1527,28 @@
         <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1570,25 +1568,25 @@
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="O9" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1608,25 +1606,25 @@
         <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="O10" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1646,25 +1644,25 @@
         <v>29</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
@@ -1684,25 +1682,25 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1722,22 +1720,22 @@
         <v>32</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1757,22 +1755,22 @@
         <v>32</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1792,22 +1790,22 @@
         <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1827,22 +1825,22 @@
         <v>32</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1862,22 +1860,22 @@
         <v>32</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1897,22 +1895,22 @@
         <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1932,22 +1930,22 @@
         <v>32</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1967,22 +1965,22 @@
         <v>32</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2002,22 +2000,22 @@
         <v>51</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2037,25 +2035,25 @@
         <v>51</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
@@ -2075,13 +2073,13 @@
         <v>56</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
@@ -2101,13 +2099,13 @@
         <v>59</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2127,25 +2125,25 @@
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="O25" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2165,22 +2163,22 @@
         <v>64</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2200,22 +2198,22 @@
         <v>64</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2229,28 +2227,28 @@
         <v>67</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2261,31 +2259,31 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>71</v>
+        <v>239</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2296,31 +2294,31 @@
         <v>1</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>73</v>
+        <v>240</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O30" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2331,31 +2329,31 @@
         <v>1</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>75</v>
+        <v>241</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2366,31 +2364,31 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O32" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2401,31 +2399,31 @@
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>80</v>
+        <v>243</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
@@ -2436,31 +2434,31 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2497,11 +2495,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D930073-A863-4E44-B413-169884B0FF0F}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2511,31 +2509,31 @@
     <col min="4" max="4" width="36.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2546,16 +2544,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2566,16 +2564,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2586,19 +2584,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>180</v>
+        <v>246</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2609,19 +2607,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>184</v>
+        <v>245</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2632,19 +2630,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2655,19 +2653,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2678,16 +2676,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2698,16 +2696,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2718,19 +2716,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2741,19 +2739,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2764,19 +2762,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2787,19 +2785,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2810,19 +2808,19 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,19 +2831,19 @@
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2856,19 +2854,19 @@
         <v>4</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2879,19 +2877,19 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2902,19 +2900,19 @@
         <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2925,42 +2923,42 @@
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="F19" s="10">
         <v>3457</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -2971,19 +2969,19 @@
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="E21" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2994,65 +2992,65 @@
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
-        <v>2</v>
+      <c r="B24" s="4" t="s">
+        <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -3060,45 +3058,45 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>236</v>
+      <c r="B26" s="4">
+        <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>215</v>
+        <v>157</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -3106,22 +3104,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -3129,22 +3127,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
@@ -3152,45 +3150,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4">
-        <v>10</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>